<commit_message>
Fixed encryption decryption fucntions
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krushivardhanreddy/Development/Python/SearchBuilder/query/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krushivardhanreddy/Development/Python/SearchBuilder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A55F46-AEAC-6540-8F2F-AC31AEB9CF18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F4B7AE-CE17-5840-AD5C-BC0F8FCAC2C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8560" yWindow="5100" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{ABFE6BB8-1EE9-44E1-BC7D-6D1EB5963869}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Schema</t>
   </si>
@@ -105,9 +105,6 @@
     <t>CNTR_MAIN</t>
   </si>
   <si>
-    <t>REVISIONS</t>
-  </si>
-  <si>
     <t>DOCUMENTS</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>DORIGINALNAME</t>
   </si>
   <si>
-    <t>DID</t>
-  </si>
-  <si>
     <t>Stellent</t>
   </si>
   <si>
@@ -139,6 +133,9 @@
   </si>
   <si>
     <t>Join</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -519,7 +516,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -561,10 +558,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +575,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -607,15 +604,18 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
+      <c r="D2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2732F657-5D10-4B06-BDD5-FA820CF75311}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -672,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -680,30 +680,16 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +729,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -751,15 +737,15 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>